<commit_message>
Atualização automática de GRAVATAI.xlsx
</commit_message>
<xml_diff>
--- a/GRAVATAI.xlsx
+++ b/GRAVATAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6917FE95-2E89-488C-A512-2563EE4EB62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F94B9C10-003C-4E22-921B-F07BC2D68DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1155,7 +1155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1216,30 +1216,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1257,7 +1233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1296,17 +1272,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1353,7 +1324,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{84136A53-7A11-4024-96DA-AB521A50BC08}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{E855C355-52D7-404D-AC9E-FD9154C0EC46}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1383,10 +1354,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35CDA2FE-7791-46E2-982D-6276EBAD3B57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{809D1930-4CE7-4425-BFE7-79B4A59F3ABF}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,7 +1395,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0832367D-0FAF-43D0-B48D-7CC3926E7440}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148A580B-B628-4F63-ACEF-A4CFB2CD8299}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1487,7 +1458,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A44299E9-9733-4FBF-9D3D-EA85BC7B655F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DB4214-6C9C-4C5A-8E28-5C618DD87629}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1506,7 +1477,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577B7450-6D23-0DAF-94F7-69A14A9D0CD0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47F678BE-55F1-DF51-3F89-74FA4A75235F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1555,7 +1526,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5B11E1-67AF-5084-6D10-9C5C47869BD5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2701C556-D3D4-92AF-461A-10A6FA4B9BF9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1574,7 +1545,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9663CDF6-BEC0-2566-70CC-D893DB9C5267}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E61A28C-47B9-3FA1-D495-0578F09F75C5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,7 +1576,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B27F88A3-983E-DD46-4AA1-E051D11420F2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C07815-6F22-1CD9-5D97-99B5E0214184}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1636,7 +1607,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72E67C63-51C1-0E1C-E724-D60DF0D6A2FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5110F384-6797-E029-EA58-1A2B7D62F3A0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1679,7 +1650,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A1EE78-ACF8-4261-A657-AE204D1EA829}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C349DCE6-D8C2-4E74-9A2A-6F211D2F1CA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1717,7 +1688,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AE0AAB4-992E-450B-A9B8-EAF41BBA9C6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA71D39-F96B-4BCF-8C6E-B856DFD82327}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1760,7 +1731,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{395A92A5-9755-438D-B1CE-0F1D415EDD5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E718998-4E77-4788-8727-1442BE467F8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2073,7 +2044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F9217C-5240-418A-A87F-313227158CAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F232EFA-D174-4DD8-9B12-342964124334}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2085,98 +2056,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5474,19 +5445,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5520,46 +5491,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5567,7 +5538,7 @@
       <c r="A2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>460433</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5579,10 +5550,10 @@
       <c r="E2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>278.39999999999998</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>480</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5621,14 +5592,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5659,79 +5630,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>302</v>
       </c>
     </row>
@@ -5756,54 +5727,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>321</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>323</v>
       </c>
     </row>
@@ -5814,43 +5786,43 @@
       <c r="B2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45108</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>4404</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>42058</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>4706</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>328</v>
       </c>
     </row>
@@ -5881,26 +5853,25 @@
       <c r="B1" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
-        <v>358</v>
-      </c>
-      <c r="F1" s="37">
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="36">
         <f>345+13</f>
         <v>358</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>2.367411718026716E-2</v>
       </c>
     </row>

</xml_diff>